<commit_message>
1. fix issue, and add some issue
</commit_message>
<xml_diff>
--- a/src/main/resources/exchange_example.xlsx
+++ b/src/main/resources/exchange_example.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freddy/workspace/gitlabsrc/wallet-java/thor-client-sdk4j/src/main/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{53E353CA-B215-5943-B072-E4AFEE0A66A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18860" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>To</t>
   </si>
@@ -34,22 +33,32 @@
     <t>BlockRef</t>
   </si>
   <si>
-    <t>0x9a</t>
-  </si>
-  <si>
     <t>0xD3EF28DF6b553eD2fc47259E8134319cB1121A2A</t>
   </si>
   <si>
     <t>交易sample</t>
   </si>
   <si>
-    <t>0x0002819f5cfc12d3</t>
+    <t>0x27</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0000695540f491a5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0000695540f491a5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xf881a94423f22ee9a0e3e1442f515f43c966b7ed</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -76,10 +85,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
+      <sz val="9"/>
       <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -221,7 +228,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -264,9 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -275,10 +279,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1429,8 +1433,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV6"/>
@@ -1439,10 +1443,10 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
@@ -1451,18 +1455,18 @@
     <col min="5" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1479,58 +1483,58 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="20.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5">
-        <v>1000.88</v>
+        <v>1.88</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9">
-        <v>1000.88</v>
+        <v>1.88</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="9">
-        <v>1000.88</v>
+        <v>1.88</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="11"/>
@@ -1543,10 +1547,16 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"1. fix issue, and add some issue"
This reverts commit a27fc8e505fc79c3b7d6d8974f7a351e6d880b92.
</commit_message>
<xml_diff>
--- a/src/main/resources/exchange_example.xlsx
+++ b/src/main/resources/exchange_example.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr date1904="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freddy/workspace/gitlabsrc/wallet-java/thor-client-sdk4j/src/main/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{53E353CA-B215-5943-B072-E4AFEE0A66A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18860" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>To</t>
   </si>
@@ -33,32 +34,22 @@
     <t>BlockRef</t>
   </si>
   <si>
+    <t>0x9a</t>
+  </si>
+  <si>
     <t>0xD3EF28DF6b553eD2fc47259E8134319cB1121A2A</t>
   </si>
   <si>
     <t>交易sample</t>
   </si>
   <si>
-    <t>0x27</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0000695540f491a5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0000695540f491a5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xf881a94423f22ee9a0e3e1442f515f43c966b7ed</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <t>0x0002819f5cfc12d3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -85,8 +76,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -228,7 +221,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -271,6 +264,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -279,10 +275,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1433,8 +1429,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV6"/>
@@ -1443,10 +1439,10 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="47.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
@@ -1455,18 +1451,18 @@
     <col min="5" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1483,58 +1479,58 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1">
+    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1000.88</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5">
-        <v>1.88</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1">
+    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1000.88</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
-        <v>1.88</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
+      <c r="D4" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1">
+    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="9">
-        <v>1.88</v>
+        <v>1000.88</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1">
+    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="11"/>
@@ -1547,16 +1543,10 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add unit test and fix some issue
</commit_message>
<xml_diff>
--- a/src/main/resources/exchange_example.xlsx
+++ b/src/main/resources/exchange_example.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freddy/workspace/gitlabsrc/wallet-java/thor-client-sdk4j/src/main/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{53E353CA-B215-5943-B072-E4AFEE0A66A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18860" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>To</t>
   </si>
@@ -34,22 +33,32 @@
     <t>BlockRef</t>
   </si>
   <si>
-    <t>0x9a</t>
-  </si>
-  <si>
     <t>0xD3EF28DF6b553eD2fc47259E8134319cB1121A2A</t>
   </si>
   <si>
     <t>交易sample</t>
   </si>
   <si>
-    <t>0x0002819f5cfc12d3</t>
+    <t>0x27</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0000695540f491a5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0000695540f491a5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xf881a94423f22ee9a0e3e1442f515f43c966b7ed</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -76,10 +85,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
+      <sz val="9"/>
       <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -221,7 +228,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -264,9 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -275,10 +279,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1429,8 +1433,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV6"/>
@@ -1439,10 +1443,10 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
@@ -1451,18 +1455,18 @@
     <col min="5" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1479,58 +1483,58 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="20.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5">
-        <v>1000.88</v>
+        <v>1.88</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9">
-        <v>1000.88</v>
+        <v>1.88</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="9">
-        <v>1000.88</v>
+        <v>1.88</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="11"/>
@@ -1543,10 +1547,16 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sign VTHO transactions console
</commit_message>
<xml_diff>
--- a/src/main/resources/exchange_example.xlsx
+++ b/src/main/resources/exchange_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>To</t>
   </si>
@@ -55,7 +55,15 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>0x0000cdb26658304d</t>
+    <t>0xD3EF28DF6b553eD2fc47259E8134319cB1121A2A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00015e41be43bb95</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00015e41be43bb95</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1447,7 +1455,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1489,16 +1497,16 @@
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5">
-        <v>1.88</v>
+        <v>188000</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1509,13 +1517,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="9">
-        <v>1.88</v>
+        <v>188000</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -1526,13 +1534,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="9">
-        <v>1.88</v>
+        <v>188000</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>

</xml_diff>